<commit_message>
optimised solution for common in 3 sorted array
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chinmay\Desktop\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2224CEE-0587-4857-A778-7C656192AB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163BB895-4C60-4CA5-8B12-F640B100967C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1918,8 +1918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2112,10 +2112,10 @@
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" ht="21">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="4"/>

</xml_diff>

<commit_message>
Brute force solution for sumarray Sum 0
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chinmay\Desktop\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72D9637-4AFD-417E-8C4B-2CF1E7C5CFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D718F19-322C-4CD9-98B9-FD1933F864E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1918,8 +1918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:B25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2130,10 +2130,10 @@
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3" ht="21">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="4"/>

</xml_diff>

<commit_message>
Edited the excel sheet
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chinmay\Desktop\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D718F19-322C-4CD9-98B9-FD1933F864E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61213971-523E-4691-9F84-6D387862963B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1918,8 +1918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2148,10 +2148,10 @@
       <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3" ht="21">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="4"/>

</xml_diff>

<commit_message>
naive solution for n/k elem in array
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chinmay\Desktop\DataStruc-Algo-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkAndStudy\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61213971-523E-4691-9F84-6D387862963B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A0258C-DDB7-480A-85B1-7C82B378483F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,7 +1919,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2157,10 +2157,10 @@
       <c r="C28" s="4"/>
     </row>
     <row r="29" spans="1:3" ht="21">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C29" s="4"/>

</xml_diff>

<commit_message>
Day 1 CodeChef boot camp
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkAndStudy\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B12FEF-F5B0-43EF-A36C-05B3AAD6F082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3243C1-6C22-4A8F-80FC-7857FDFEADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1423,7 +1423,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1540,6 +1540,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1562,7 +1578,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1601,6 +1617,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1919,7 +1939,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:B30"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2166,10 +2186,10 @@
       <c r="C29" s="4"/>
     </row>
     <row r="30" spans="1:3" ht="21">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C30" s="4"/>

</xml_diff>

<commit_message>
Brute force for is a subset or not
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkAndStudy\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06812B04-D4FA-4EB2-9A7B-FE378D4C86FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF760E2-61C9-42AF-B443-4D744FAA24AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1939,7 +1939,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:B31"/>
+      <selection activeCell="A32" sqref="A32:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2204,10 +2204,10 @@
       <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:3" ht="21">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C32" s="4"/>

</xml_diff>

<commit_message>
O(n^2) for  finding the triplet
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkAndStudy\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF760E2-61C9-42AF-B443-4D744FAA24AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E425BCA-CAF3-4C34-A822-BFEF2049D9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1938,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:B32"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2213,10 +2213,10 @@
       <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:3" ht="21">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="4"/>

</xml_diff>

<commit_message>
Stated rainWaterProblem Updated excel sheet
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkAndStudy\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E425BCA-CAF3-4C34-A822-BFEF2049D9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80A75A3-4D51-464C-896E-E06C2555AB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1939,7 +1939,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:B33"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2222,10 +2222,10 @@
       <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3" ht="21">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C34" s="4"/>

</xml_diff>

<commit_message>
updated excel sheet and started choc dis problem
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkAndStudy\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80A75A3-4D51-464C-896E-E06C2555AB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD87F66-AF0B-4C4D-A7E2-380033834E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1939,7 +1939,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A35" sqref="A35:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2231,10 +2231,10 @@
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" ht="21">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C35" s="4"/>

</xml_diff>

<commit_message>
Median code giving RUNTIME ERROR
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkAndStudy\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A91019-515A-4580-8155-DF11DAE7BCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6FA333-D978-43F2-B4C5-28D514F98A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3048" yWindow="1392" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1423,7 +1423,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1556,6 +1556,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1578,7 +1594,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1621,6 +1637,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1938,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2285,10 +2305,10 @@
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:3" ht="21">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="21" t="s">
         <v>38</v>
       </c>
       <c r="C41" s="4"/>

</xml_diff>

<commit_message>
Spiral traversal of a matrix
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkAndStudy\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6FA333-D978-43F2-B4C5-28D514F98A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D9FB95-FC8E-46E1-93D2-EE0FB06BB906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3048" yWindow="1392" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1958,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2323,10 +2323,10 @@
       <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C44" s="4"/>

</xml_diff>

<commit_message>
Updated excel sheet and optimised Search in mat
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkAndStudy\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D9FB95-FC8E-46E1-93D2-EE0FB06BB906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB723C6-AAEA-455F-9DD0-95CFDE89533A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3048" yWindow="1392" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1958,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:B44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2332,10 +2332,10 @@
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" ht="21">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C45" s="4"/>

</xml_diff>

<commit_message>
Brute force for max number of ones
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkAndStudy\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB723C6-AAEA-455F-9DD0-95CFDE89533A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8A91A7-0009-4C64-8F97-DBFB17E5CA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3048" yWindow="1392" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1958,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:B45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2341,10 +2341,10 @@
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3" ht="21">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="19" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="4"/>

</xml_diff>

<commit_message>
maximal rec in matrix
</commit_message>
<xml_diff>
--- a/DSAquestionSheet.xlsx
+++ b/DSAquestionSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkAndStudy\DataStruc-Algo-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBE18F7-C1C2-44DE-BC4F-A0F9F3D4AB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D490E247-3EBB-4A24-BE4D-959F775CD4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3048" yWindow="1392" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1959,7 +1959,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:B48"/>
+      <selection activeCell="A49" sqref="A49:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2368,10 +2368,10 @@
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="1:3" ht="21">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="21" t="s">
         <v>45</v>
       </c>
       <c r="C49" s="4"/>

</xml_diff>